<commit_message>
updated open cv error
</commit_message>
<xml_diff>
--- a/match_results.xlsx
+++ b/match_results.xlsx
@@ -1,13 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -481,24 +481,24 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>image_3_2.png</t>
+          <t>image_0_2.png</t>
         </is>
       </c>
       <c r="C2" t="n">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="D2" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>Paw yellow</t>
+          <t>3 inch white drizzle bone</t>
         </is>
       </c>
       <c r="F2" t="inlineStr"/>
       <c r="G2" t="inlineStr">
         <is>
-          <t>ABC126</t>
+          <t>ABC123</t>
         </is>
       </c>
       <c r="H2" t="inlineStr"/>
@@ -513,7 +513,7 @@
         </is>
       </c>
       <c r="C3" t="n">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="D3" t="n">
         <v>2</v>

</xml_diff>